<commit_message>
📝 Update time schedule
</commit_message>
<xml_diff>
--- a/docs/assets/03-time.xlsx
+++ b/docs/assets/03-time.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10520"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{596561B2-8AB8-E146-ADD4-C1EF7971439A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD05D02-82E3-AF42-872C-2F1200CE7B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t xml:space="preserve"> Hervorgehobener Zeitraum:</t>
   </si>
@@ -170,9 +170,6 @@
     <t>Gantt Diagramm erstellen</t>
   </si>
   <si>
-    <t>GitHub Kanban aufsetzen</t>
-  </si>
-  <si>
     <t>GitHub / TypeScript aufsetzen</t>
   </si>
   <si>
@@ -213,7 +210,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -317,6 +314,14 @@
       <b/>
       <sz val="13"/>
       <color theme="1" tint="0.24994659260841701"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="13"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -507,7 +512,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -618,6 +623,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1028,10 +1036,10 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:BO30"/>
+  <dimension ref="B1:BO26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="108" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1278,7 +1286,9 @@
       <c r="E6" s="7">
         <v>1</v>
       </c>
-      <c r="F6" s="7"/>
+      <c r="F6" s="7">
+        <v>3</v>
+      </c>
       <c r="G6" s="8">
         <v>0.66</v>
       </c>
@@ -1311,13 +1321,15 @@
       <c r="D8" s="7">
         <v>2</v>
       </c>
-      <c r="E8" s="7"/>
+      <c r="E8" s="7">
+        <v>2</v>
+      </c>
       <c r="F8" s="7"/>
       <c r="G8" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:67" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
         <v>18</v>
       </c>
@@ -1325,111 +1337,135 @@
         <v>1</v>
       </c>
       <c r="D9" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E9" s="7">
         <v>2</v>
       </c>
       <c r="F9" s="7">
+        <v>2</v>
+      </c>
+      <c r="G9" s="8">
         <v>1</v>
       </c>
-      <c r="G9" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:67" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="6" t="s">
+    </row>
+    <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="24" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D10" s="7">
+        <v>2</v>
+      </c>
+      <c r="E10" s="7">
         <v>3</v>
       </c>
-      <c r="E10" s="7">
+      <c r="F10" s="7">
         <v>2</v>
       </c>
-      <c r="F10" s="7"/>
       <c r="G10" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="6"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
+      <c r="B11" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="7">
+        <v>4</v>
+      </c>
+      <c r="D11" s="7">
+        <v>2</v>
+      </c>
+      <c r="E11" s="7">
+        <v>8</v>
+      </c>
       <c r="F11" s="7"/>
-      <c r="G11" s="8"/>
-    </row>
-    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G11" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:67" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="24" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C12" s="7">
+        <v>5</v>
+      </c>
+      <c r="D12" s="7">
+        <v>1</v>
+      </c>
+      <c r="E12" s="7">
         <v>3</v>
       </c>
-      <c r="D12" s="7">
-        <v>2</v>
-      </c>
-      <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:67" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="7">
-        <v>4</v>
+        <v>22</v>
+      </c>
+      <c r="C13" s="9">
+        <v>5</v>
       </c>
       <c r="D13" s="7">
         <v>2</v>
       </c>
-      <c r="E13" s="7"/>
+      <c r="E13" s="7">
+        <v>4</v>
+      </c>
       <c r="F13" s="7"/>
       <c r="G13" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:67" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:67" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="24" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C14" s="7">
+        <v>6</v>
+      </c>
+      <c r="D14" s="7">
+        <v>2</v>
+      </c>
+      <c r="E14" s="7">
         <v>5</v>
       </c>
-      <c r="D14" s="7">
-        <v>1</v>
-      </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
+      <c r="F14" s="7">
+        <v>4</v>
+      </c>
       <c r="G14" s="8">
-        <v>0</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="15" spans="2:67" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="9">
-        <v>5</v>
+        <v>24</v>
+      </c>
+      <c r="C15" s="7">
+        <v>7</v>
       </c>
       <c r="D15" s="7">
         <v>2</v>
       </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
+      <c r="E15" s="7">
+        <v>6</v>
+      </c>
+      <c r="F15" s="7">
+        <v>1</v>
+      </c>
       <c r="G15" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:67" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="24" t="s">
-        <v>24</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:67" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="37" t="s">
+        <v>25</v>
       </c>
       <c r="C16" s="7">
         <v>6</v>
@@ -1443,47 +1479,53 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="24" t="s">
-        <v>25</v>
+    <row r="17" spans="2:7" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="37" t="s">
+        <v>27</v>
       </c>
       <c r="C17" s="7">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D17" s="7">
+        <v>4</v>
+      </c>
+      <c r="E17" s="7">
+        <v>8</v>
+      </c>
+      <c r="F17" s="7">
         <v>2</v>
       </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
       <c r="G17" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="24" t="s">
         <v>26</v>
       </c>
       <c r="C18" s="7">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D18" s="7">
-        <v>2</v>
-      </c>
-      <c r="E18" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="E18" s="7">
+        <v>9</v>
+      </c>
       <c r="F18" s="7"/>
       <c r="G18" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="24" t="s">
         <v>28</v>
       </c>
       <c r="C19" s="7">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D19" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
@@ -1492,9 +1534,15 @@
       </c>
     </row>
     <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="24"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
+      <c r="B20" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="7">
+        <v>11</v>
+      </c>
+      <c r="D20" s="7">
+        <v>2</v>
+      </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
       <c r="G20" s="8">
@@ -1502,31 +1550,19 @@
       </c>
     </row>
     <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="7">
-        <v>9</v>
-      </c>
-      <c r="D21" s="7">
-        <v>1</v>
-      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="G21" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="7">
-        <v>9</v>
-      </c>
-      <c r="D22" s="7">
-        <v>3</v>
-      </c>
+    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="6"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="8">
@@ -1544,15 +1580,9 @@
       </c>
     </row>
     <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" s="7">
-        <v>11</v>
-      </c>
-      <c r="D24" s="7">
-        <v>2</v>
-      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
       <c r="G24" s="8">
@@ -1576,46 +1606,6 @@
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="6"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="6"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="6"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="6"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1633,7 +1623,7 @@
     <mergeCell ref="V2:Y2"/>
     <mergeCell ref="AA2:AG2"/>
   </mergeCells>
-  <conditionalFormatting sqref="H5:BO30">
+  <conditionalFormatting sqref="H5:BO26">
     <cfRule type="expression" dxfId="9" priority="1">
       <formula>ProzentAbgeschlossen</formula>
     </cfRule>
@@ -1659,7 +1649,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B31:BO31">
+  <conditionalFormatting sqref="B27:BO27">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>TRUE</formula>
     </cfRule>
@@ -1704,6 +1694,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100A0B9B8EFB60403439C9E81A048B1B583" ma:contentTypeVersion="2" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="c84d8dd099a1334dea1db973fa611002">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8a1c7d89-dfaa-462a-9ab2-70ad922e6806" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cb7cef8f59a6b9ad3346908c5f99d9b1" ns2:_="">
     <xsd:import namespace="8a1c7d89-dfaa-462a-9ab2-70ad922e6806"/>
@@ -1835,12 +1831,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1851,6 +1841,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C957879-AD63-4472-AE0F-E2E0120ADCCF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABE0C6CF-A046-4C24-A91F-E73669FB03F6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1868,15 +1867,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C957879-AD63-4472-AE0F-E2E0120ADCCF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70B927A1-3D68-48F6-B958-B6DB28B89C1F}">
   <ds:schemaRefs>

</xml_diff>